<commit_message>
added extra boolean queries
</commit_message>
<xml_diff>
--- a/results/datasheets/search-results.xlsx
+++ b/results/datasheets/search-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="5000" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="16">
   <si>
     <t xml:space="preserve">AND</t>
   </si>
@@ -51,6 +51,12 @@
     <t xml:space="preserve">(call || enron) &amp;&amp; (time || attach) &amp;&amp; (inform || work) &amp;&amp; (meet || week)</t>
   </si>
   <si>
+    <t xml:space="preserve">(call &amp;&amp; enron) || (time &amp;&amp; attach)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(call &amp;&amp; enron) || (time &amp;&amp; attach) || (inform &amp;&amp; work) || (meet &amp;&amp; week)</t>
+  </si>
+  <si>
     <t xml:space="preserve">!enron &amp;&amp; !time</t>
   </si>
   <si>
@@ -73,7 +79,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -104,12 +110,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -134,10 +134,52 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -168,7 +210,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -177,11 +219,51 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -257,7 +339,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -280,7 +362,6 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -290,9 +371,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'5000'!$F$29:$Q$29</c:f>
+              <c:f>'5000'!$F$29:$S$29</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2 words</c:v>
                 </c:pt>
@@ -318,15 +399,21 @@
                   <c:v>(call || enron) &amp;&amp; (time || attach) &amp;&amp; (inform || work) &amp;&amp; (meet || week)</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>(call &amp;&amp; enron) || (time &amp;&amp; attach)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(call &amp;&amp; enron) || (time &amp;&amp; attach) || (inform &amp;&amp; work) || (meet &amp;&amp; week)</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>!enron &amp;&amp; !time</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>!(enron &amp;&amp; time)</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>!enron || !time</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>!(enron || time)</c:v>
                 </c:pt>
               </c:strCache>
@@ -334,10 +421,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'5000'!$F$31:$Q$31</c:f>
+              <c:f>'5000'!$F$31:$S$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0.0271666666666667</c:v>
                 </c:pt>
@@ -363,15 +450,21 @@
                   <c:v>0.0963333333333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0.0503333333333333</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.081</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.045</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>0.0268333333333333</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>0.0463333333333333</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>0.028</c:v>
                 </c:pt>
               </c:numCache>
@@ -380,11 +473,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="97526461"/>
-        <c:axId val="23640582"/>
+        <c:axId val="82643858"/>
+        <c:axId val="55946521"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="97526461"/>
+        <c:axId val="82643858"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -419,14 +512,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23640582"/>
+        <c:crossAx val="55946521"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="23640582"/>
+        <c:axId val="55946521"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -441,7 +534,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -470,7 +563,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97526461"/>
+        <c:crossAx val="82643858"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -507,12 +600,23 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0515545590433483"/>
+          <c:y val="0.0613723540275607"/>
+          <c:w val="0.881644245142003"/>
+          <c:h val="0.359283989203012"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -530,7 +634,6 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -540,9 +643,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'10000'!$E$23:$P$23</c:f>
+              <c:f>'10000'!$E$23:$R$23</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2 words</c:v>
                 </c:pt>
@@ -568,15 +671,21 @@
                   <c:v>(call || enron) &amp;&amp; (time || attach) &amp;&amp; (inform || work) &amp;&amp; (meet || week)</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>(call &amp;&amp; enron) || (time &amp;&amp; attach)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(call &amp;&amp; enron) || (time &amp;&amp; attach) || (inform &amp;&amp; work) || (meet &amp;&amp; week)</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>!enron &amp;&amp; !time</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>!(enron &amp;&amp; time)</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>!enron || !time</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>!(enron || time)</c:v>
                 </c:pt>
               </c:strCache>
@@ -584,10 +693,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'10000'!$E$25:$P$25</c:f>
+              <c:f>'10000'!$E$25:$R$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0.0633333333333333</c:v>
                 </c:pt>
@@ -613,15 +722,21 @@
                   <c:v>0.234</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0.124</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.194</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.133666666666667</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>0.064</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>0.136166666666667</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>0.065</c:v>
                 </c:pt>
               </c:numCache>
@@ -630,11 +745,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="40774833"/>
-        <c:axId val="81418229"/>
+        <c:axId val="44984030"/>
+        <c:axId val="7264917"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="40774833"/>
+        <c:axId val="44984030"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -669,14 +784,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81418229"/>
+        <c:crossAx val="7264917"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81418229"/>
+        <c:axId val="7264917"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -691,7 +806,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -720,7 +835,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40774833"/>
+        <c:crossAx val="44984030"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -757,7 +872,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -780,7 +895,6 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -790,9 +904,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'15000'!$G$31:$R$31</c:f>
+              <c:f>'15000'!$G$31:$T$31</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2 words</c:v>
                 </c:pt>
@@ -818,15 +932,21 @@
                   <c:v>(call || enron) &amp;&amp; (time || attach) &amp;&amp; (inform || work) &amp;&amp; (meet || week)</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>(call &amp;&amp; enron) || (time &amp;&amp; attach)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(call &amp;&amp; enron) || (time &amp;&amp; attach) || (inform &amp;&amp; work) || (meet &amp;&amp; week)</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>!enron &amp;&amp; !time</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>!(enron &amp;&amp; time)</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>!enron || !time</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>!(enron || time)</c:v>
                 </c:pt>
               </c:strCache>
@@ -834,10 +954,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'15000'!$G$33:$R$33</c:f>
+              <c:f>'15000'!$G$33:$T$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0.0986</c:v>
                 </c:pt>
@@ -863,15 +983,21 @@
                   <c:v>0.4045</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0.1825</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.304</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.2588</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>0.0985</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>0.2625</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>0.105</c:v>
                 </c:pt>
               </c:numCache>
@@ -880,11 +1006,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="76839567"/>
-        <c:axId val="69716751"/>
+        <c:axId val="52082235"/>
+        <c:axId val="43719508"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76839567"/>
+        <c:axId val="52082235"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -919,14 +1045,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69716751"/>
+        <c:crossAx val="43719508"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69716751"/>
+        <c:axId val="43719508"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -941,7 +1067,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -970,7 +1096,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76839567"/>
+        <c:crossAx val="52082235"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1011,16 +1137,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>194040</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>609480</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>263880</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>96840</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>93240</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>9360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1028,8 +1154,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6756480" y="5960880"/>
-        <a:ext cx="5670720" cy="3239280"/>
+        <a:off x="3895560" y="5855760"/>
+        <a:ext cx="9222120" cy="5695200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1047,15 +1173,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>522000</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>122040</xdr:rowOff>
+      <xdr:colOff>49680</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>591480</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>375840</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>143640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1063,8 +1189,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4522320" y="4511160"/>
-        <a:ext cx="5670360" cy="3239280"/>
+        <a:off x="3954600" y="4341240"/>
+        <a:ext cx="12042000" cy="5068080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1081,16 +1207,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>65880</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>105120</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>14760</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>97560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1919880</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>93240</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>349200</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>86760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1098,8 +1224,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8114400" y="5794560"/>
-        <a:ext cx="5692680" cy="3239280"/>
+        <a:off x="4615200" y="6112080"/>
+        <a:ext cx="14031360" cy="4541040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1117,17 +1243,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="E4:R31"/>
+  <dimension ref="E4:T31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topLeft" activeCell="M26" activeCellId="0" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.2551020408163"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="28.2040816326531"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1150,432 +1276,496 @@
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2" t="s">
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2" t="s">
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="Q8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="R8" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="S8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T8" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="G9" s="5" t="n">
         <v>440</v>
       </c>
-      <c r="H9" s="3" t="n">
+      <c r="H9" s="6" t="n">
         <v>48</v>
       </c>
-      <c r="I9" s="3" t="n">
+      <c r="I9" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="J9" s="3" t="n">
+      <c r="J9" s="8" t="n">
         <v>1945</v>
       </c>
-      <c r="K9" s="3" t="n">
+      <c r="K9" s="6" t="n">
         <v>2835</v>
       </c>
-      <c r="L9" s="3" t="n">
+      <c r="L9" s="9" t="n">
         <v>3366</v>
       </c>
-      <c r="M9" s="3" t="n">
+      <c r="M9" s="8" t="n">
         <v>976</v>
       </c>
-      <c r="N9" s="3" t="n">
+      <c r="N9" s="6" t="n">
         <v>263</v>
       </c>
-      <c r="O9" s="3" t="n">
+      <c r="O9" s="6" t="n">
+        <v>518</v>
+      </c>
+      <c r="P9" s="9" t="n">
+        <v>796</v>
+      </c>
+      <c r="Q9" s="6" t="n">
         <v>3023</v>
       </c>
-      <c r="P9" s="3" t="n">
+      <c r="R9" s="6" t="n">
         <v>4528</v>
       </c>
-      <c r="Q9" s="3" t="n">
+      <c r="S9" s="6" t="n">
         <v>4528</v>
       </c>
-      <c r="R9" s="3" t="n">
+      <c r="T9" s="6" t="n">
         <v>3023</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="10" t="n">
         <v>0.029</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>0.059</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10" s="11" t="n">
         <v>0.093</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="J10" s="12" t="n">
         <v>0.034</v>
       </c>
       <c r="K10" s="0" t="n">
         <v>0.078</v>
       </c>
-      <c r="L10" s="0" t="n">
+      <c r="L10" s="13" t="n">
         <v>0.173</v>
       </c>
-      <c r="M10" s="0" t="n">
+      <c r="M10" s="12" t="n">
         <v>0.058</v>
       </c>
       <c r="N10" s="0" t="n">
         <v>0.093</v>
       </c>
       <c r="O10" s="0" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="P10" s="13" t="n">
+        <v>0.082</v>
+      </c>
+      <c r="Q10" s="0" t="n">
         <v>0.045</v>
       </c>
-      <c r="P10" s="0" t="n">
+      <c r="R10" s="0" t="n">
         <v>0.028</v>
       </c>
-      <c r="Q10" s="0" t="n">
+      <c r="S10" s="0" t="n">
         <v>0.046</v>
       </c>
-      <c r="R10" s="0" t="n">
+      <c r="T10" s="0" t="n">
         <v>0.027</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="10" t="n">
         <v>0.026</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>0.056</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I11" s="11" t="n">
         <v>0.086</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="J11" s="12" t="n">
         <v>0.029</v>
       </c>
       <c r="K11" s="0" t="n">
         <v>0.081</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="L11" s="13" t="n">
         <v>0.17</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="M11" s="12" t="n">
         <v>0.058</v>
       </c>
       <c r="N11" s="0" t="n">
         <v>0.098</v>
       </c>
       <c r="O11" s="0" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="P11" s="13" t="n">
+        <v>0.084</v>
+      </c>
+      <c r="Q11" s="0" t="n">
         <v>0.045</v>
       </c>
-      <c r="P11" s="0" t="n">
+      <c r="R11" s="0" t="n">
         <v>0.027</v>
       </c>
-      <c r="Q11" s="0" t="n">
+      <c r="S11" s="0" t="n">
         <v>0.046</v>
       </c>
-      <c r="R11" s="0" t="n">
+      <c r="T11" s="0" t="n">
         <v>0.029</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="10" t="n">
         <v>0.027</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>0.058</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I12" s="11" t="n">
         <v>0.108</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="J12" s="12" t="n">
         <v>0.033</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>0.079</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="L12" s="13" t="n">
         <v>0.169</v>
       </c>
-      <c r="M12" s="0" t="n">
+      <c r="M12" s="12" t="n">
         <v>0.059</v>
       </c>
       <c r="N12" s="0" t="n">
         <v>0.096</v>
       </c>
       <c r="O12" s="0" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="P12" s="13" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="Q12" s="0" t="n">
         <v>0.045</v>
       </c>
-      <c r="P12" s="0" t="n">
+      <c r="R12" s="0" t="n">
         <v>0.027</v>
       </c>
-      <c r="Q12" s="0" t="n">
+      <c r="S12" s="0" t="n">
         <v>0.047</v>
       </c>
-      <c r="R12" s="0" t="n">
+      <c r="T12" s="0" t="n">
         <v>0.029</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="10" t="n">
         <v>0.027</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>0.058</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="I13" s="11" t="n">
         <v>0.097</v>
       </c>
-      <c r="J13" s="0" t="n">
+      <c r="J13" s="12" t="n">
         <v>0.029</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>0.079</v>
       </c>
-      <c r="L13" s="0" t="n">
+      <c r="L13" s="13" t="n">
         <v>0.17</v>
       </c>
-      <c r="M13" s="0" t="n">
+      <c r="M13" s="12" t="n">
         <v>0.06</v>
       </c>
       <c r="N13" s="0" t="n">
         <v>0.096</v>
       </c>
       <c r="O13" s="0" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="P13" s="13" t="n">
+        <v>0.082</v>
+      </c>
+      <c r="Q13" s="0" t="n">
         <v>0.045</v>
       </c>
-      <c r="P13" s="0" t="n">
+      <c r="R13" s="0" t="n">
         <v>0.026</v>
       </c>
-      <c r="Q13" s="0" t="n">
+      <c r="S13" s="0" t="n">
         <v>0.046</v>
       </c>
-      <c r="R13" s="0" t="n">
+      <c r="T13" s="0" t="n">
         <v>0.028</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="10" t="n">
         <v>0.027</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>0.059</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="I14" s="11" t="n">
         <v>0.1</v>
       </c>
-      <c r="J14" s="0" t="n">
+      <c r="J14" s="12" t="n">
         <v>0.027</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>0.08</v>
       </c>
-      <c r="L14" s="0" t="n">
+      <c r="L14" s="13" t="n">
         <v>0.168</v>
       </c>
-      <c r="M14" s="0" t="n">
+      <c r="M14" s="12" t="n">
         <v>0.059</v>
       </c>
       <c r="N14" s="0" t="n">
         <v>0.098</v>
       </c>
       <c r="O14" s="0" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="P14" s="13" t="n">
+        <v>0.079</v>
+      </c>
+      <c r="Q14" s="0" t="n">
         <v>0.045</v>
       </c>
-      <c r="P14" s="0" t="n">
+      <c r="R14" s="0" t="n">
         <v>0.027</v>
       </c>
-      <c r="Q14" s="0" t="n">
+      <c r="S14" s="0" t="n">
         <v>0.047</v>
       </c>
-      <c r="R14" s="0" t="n">
+      <c r="T14" s="0" t="n">
         <v>0.028</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="10" t="n">
         <v>0.027</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>0.062</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I15" s="11" t="n">
         <v>0.094</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="J15" s="12" t="n">
         <v>0.034</v>
       </c>
       <c r="K15" s="0" t="n">
         <v>0.083</v>
       </c>
-      <c r="L15" s="0" t="n">
+      <c r="L15" s="13" t="n">
         <v>0.175</v>
       </c>
-      <c r="M15" s="0" t="n">
+      <c r="M15" s="12" t="n">
         <v>0.062</v>
       </c>
       <c r="N15" s="0" t="n">
         <v>0.097</v>
       </c>
       <c r="O15" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="P15" s="13" t="n">
+        <v>0.081</v>
+      </c>
+      <c r="Q15" s="0" t="n">
         <v>0.045</v>
       </c>
-      <c r="P15" s="0" t="n">
+      <c r="R15" s="0" t="n">
         <v>0.026</v>
       </c>
-      <c r="Q15" s="0" t="n">
+      <c r="S15" s="0" t="n">
         <v>0.046</v>
       </c>
-      <c r="R15" s="0" t="n">
+      <c r="T15" s="0" t="n">
         <v>0.027</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2" t="s">
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2" t="s">
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2" t="s">
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="I29" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J29" s="3" t="s">
+      <c r="J29" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="K29" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L29" s="3" t="s">
+      <c r="L29" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="M29" s="3" t="s">
+      <c r="M29" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N29" s="3" t="s">
+      <c r="N29" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="O29" s="3" t="s">
+      <c r="O29" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="P29" s="3" t="s">
+      <c r="P29" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="Q29" s="3" t="s">
+      <c r="Q29" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="R29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S29" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E30" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="F30" s="8" t="n">
         <v>440</v>
       </c>
-      <c r="G30" s="3" t="n">
+      <c r="G30" s="6" t="n">
         <v>48</v>
       </c>
-      <c r="H30" s="3" t="n">
+      <c r="H30" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="I30" s="3" t="n">
+      <c r="I30" s="6" t="n">
         <v>1945</v>
       </c>
-      <c r="J30" s="3" t="n">
+      <c r="J30" s="6" t="n">
         <v>2835</v>
       </c>
-      <c r="K30" s="3" t="n">
+      <c r="K30" s="6" t="n">
         <v>3366</v>
       </c>
-      <c r="L30" s="3" t="n">
+      <c r="L30" s="8" t="n">
         <v>976</v>
       </c>
-      <c r="M30" s="3" t="n">
+      <c r="M30" s="6" t="n">
         <v>263</v>
       </c>
-      <c r="N30" s="3" t="n">
+      <c r="N30" s="6" t="n">
+        <v>518</v>
+      </c>
+      <c r="O30" s="9" t="n">
+        <v>796</v>
+      </c>
+      <c r="P30" s="6" t="n">
         <v>3023</v>
       </c>
-      <c r="O30" s="3" t="n">
+      <c r="Q30" s="6" t="n">
         <v>4528</v>
       </c>
-      <c r="P30" s="3" t="n">
+      <c r="R30" s="6" t="n">
         <v>4528</v>
       </c>
-      <c r="Q30" s="3" t="n">
+      <c r="S30" s="6" t="n">
         <v>3023</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F31" s="0" t="n">
+      <c r="F31" s="12" t="n">
         <f aca="false">AVERAGE(G10:G15)</f>
         <v>0.0271666666666667</v>
       </c>
@@ -1583,7 +1773,7 @@
         <f aca="false">AVERAGE(H10:H15)</f>
         <v>0.0586666666666667</v>
       </c>
-      <c r="H31" s="0" t="n">
+      <c r="H31" s="13" t="n">
         <f aca="false">AVERAGE(I10:I15)</f>
         <v>0.0963333333333333</v>
       </c>
@@ -1599,7 +1789,7 @@
         <f aca="false">AVERAGE(L10:L15)</f>
         <v>0.170833333333333</v>
       </c>
-      <c r="L31" s="0" t="n">
+      <c r="L31" s="12" t="n">
         <f aca="false">AVERAGE(M10:M15)</f>
         <v>0.0593333333333333</v>
       </c>
@@ -1609,18 +1799,26 @@
       </c>
       <c r="N31" s="0" t="n">
         <f aca="false">AVERAGE(O10:O15)</f>
-        <v>0.045</v>
-      </c>
-      <c r="O31" s="0" t="n">
+        <v>0.0503333333333333</v>
+      </c>
+      <c r="O31" s="13" t="n">
         <f aca="false">AVERAGE(P10:P15)</f>
-        <v>0.0268333333333333</v>
+        <v>0.081</v>
       </c>
       <c r="P31" s="0" t="n">
         <f aca="false">AVERAGE(Q10:Q15)</f>
-        <v>0.0463333333333333</v>
+        <v>0.045</v>
       </c>
       <c r="Q31" s="0" t="n">
         <f aca="false">AVERAGE(R10:R15)</f>
+        <v>0.0268333333333333</v>
+      </c>
+      <c r="R31" s="0" t="n">
+        <f aca="false">AVERAGE(S10:S15)</f>
+        <v>0.0463333333333333</v>
+      </c>
+      <c r="S31" s="0" t="n">
+        <f aca="false">AVERAGE(T10:T15)</f>
         <v>0.028</v>
       </c>
     </row>
@@ -1632,12 +1830,12 @@
     <mergeCell ref="M4:P4"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:R7"/>
+    <mergeCell ref="M7:P7"/>
+    <mergeCell ref="Q7:T7"/>
     <mergeCell ref="F28:H28"/>
     <mergeCell ref="I28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="N28:Q28"/>
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="P28:S28"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1655,126 +1853,137 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="D4:Q25"/>
+  <dimension ref="D4:S25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q18" activeCellId="0" sqref="Q18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2" t="s">
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2" t="s">
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="Q5" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="F6" s="8" t="n">
         <v>869</v>
       </c>
-      <c r="G6" s="3" t="n">
+      <c r="G6" s="6" t="n">
         <v>90</v>
       </c>
-      <c r="H6" s="3" t="n">
+      <c r="H6" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="I6" s="3" t="n">
+      <c r="I6" s="6" t="n">
         <v>3995</v>
       </c>
-      <c r="J6" s="3" t="n">
+      <c r="J6" s="6" t="n">
         <v>5861</v>
       </c>
-      <c r="K6" s="3" t="n">
+      <c r="K6" s="6" t="n">
         <v>6867</v>
       </c>
-      <c r="L6" s="3" t="n">
+      <c r="L6" s="8" t="n">
         <v>1958</v>
       </c>
-      <c r="M6" s="3" t="n">
+      <c r="M6" s="6" t="n">
         <v>554</v>
       </c>
-      <c r="N6" s="3" t="n">
+      <c r="N6" s="6" t="n">
+        <v>1078</v>
+      </c>
+      <c r="O6" s="9" t="n">
+        <v>1637</v>
+      </c>
+      <c r="P6" s="6" t="n">
         <v>5910</v>
       </c>
-      <c r="O6" s="3" t="n">
+      <c r="Q6" s="6" t="n">
         <v>9036</v>
       </c>
-      <c r="P6" s="3" t="n">
+      <c r="R6" s="6" t="n">
         <v>9036</v>
       </c>
-      <c r="Q6" s="3" t="n">
+      <c r="S6" s="6" t="n">
         <v>5910</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="12" t="n">
         <v>0.064</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>0.125</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="13" t="n">
         <v>0.194</v>
       </c>
       <c r="I7" s="0" t="n">
@@ -1786,33 +1995,39 @@
       <c r="K7" s="0" t="n">
         <v>0.541</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="L7" s="12" t="n">
         <v>0.141</v>
       </c>
       <c r="M7" s="0" t="n">
         <v>0.235</v>
       </c>
       <c r="N7" s="0" t="n">
+        <v>0.117</v>
+      </c>
+      <c r="O7" s="13" t="n">
+        <v>0.196</v>
+      </c>
+      <c r="P7" s="0" t="n">
         <v>0.131</v>
       </c>
-      <c r="O7" s="0" t="n">
+      <c r="Q7" s="0" t="n">
         <v>0.066</v>
       </c>
-      <c r="P7" s="0" t="n">
+      <c r="R7" s="0" t="n">
         <v>0.134</v>
       </c>
-      <c r="Q7" s="0" t="n">
+      <c r="S7" s="0" t="n">
         <v>0.063</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="12" t="n">
         <v>0.065</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>0.123</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="13" t="n">
         <v>0.185</v>
       </c>
       <c r="I8" s="0" t="n">
@@ -1824,33 +2039,39 @@
       <c r="K8" s="0" t="n">
         <v>0.542</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="L8" s="12" t="n">
         <v>0.14</v>
       </c>
       <c r="M8" s="0" t="n">
         <v>0.231</v>
       </c>
       <c r="N8" s="0" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="O8" s="13" t="n">
+        <v>0.191</v>
+      </c>
+      <c r="P8" s="0" t="n">
         <v>0.129</v>
       </c>
-      <c r="O8" s="0" t="n">
+      <c r="Q8" s="0" t="n">
         <v>0.066</v>
       </c>
-      <c r="P8" s="0" t="n">
+      <c r="R8" s="0" t="n">
         <v>0.136</v>
       </c>
-      <c r="Q8" s="0" t="n">
+      <c r="S8" s="0" t="n">
         <v>0.064</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="12" t="n">
         <v>0.064</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>0.119</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="13" t="n">
         <v>0.188</v>
       </c>
       <c r="I9" s="0" t="n">
@@ -1862,33 +2083,39 @@
       <c r="K9" s="0" t="n">
         <v>0.544</v>
       </c>
-      <c r="L9" s="0" t="n">
+      <c r="L9" s="12" t="n">
         <v>0.139</v>
       </c>
       <c r="M9" s="0" t="n">
         <v>0.235</v>
       </c>
       <c r="N9" s="0" t="n">
+        <v>0.153</v>
+      </c>
+      <c r="O9" s="13" t="n">
+        <v>0.194</v>
+      </c>
+      <c r="P9" s="0" t="n">
         <v>0.132</v>
       </c>
-      <c r="O9" s="0" t="n">
+      <c r="Q9" s="0" t="n">
         <v>0.064</v>
       </c>
-      <c r="P9" s="0" t="n">
+      <c r="R9" s="0" t="n">
         <v>0.137</v>
       </c>
-      <c r="Q9" s="0" t="n">
+      <c r="S9" s="0" t="n">
         <v>0.065</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="12" t="n">
         <v>0.063</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>0.124</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="13" t="n">
         <v>0.191</v>
       </c>
       <c r="I10" s="0" t="n">
@@ -1900,33 +2127,39 @@
       <c r="K10" s="0" t="n">
         <v>0.556</v>
       </c>
-      <c r="L10" s="0" t="n">
+      <c r="L10" s="12" t="n">
         <v>0.143</v>
       </c>
       <c r="M10" s="0" t="n">
         <v>0.237</v>
       </c>
       <c r="N10" s="0" t="n">
+        <v>0.109</v>
+      </c>
+      <c r="O10" s="13" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="P10" s="0" t="n">
         <v>0.148</v>
       </c>
-      <c r="O10" s="0" t="n">
+      <c r="Q10" s="0" t="n">
         <v>0.065</v>
       </c>
-      <c r="P10" s="0" t="n">
+      <c r="R10" s="0" t="n">
         <v>0.135</v>
       </c>
-      <c r="Q10" s="0" t="n">
+      <c r="S10" s="0" t="n">
         <v>0.064</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="12" t="n">
         <v>0.061</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>0.128</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="13" t="n">
         <v>0.189</v>
       </c>
       <c r="I11" s="0" t="n">
@@ -1938,33 +2171,39 @@
       <c r="K11" s="0" t="n">
         <v>0.532</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="L11" s="12" t="n">
         <v>0.141</v>
       </c>
       <c r="M11" s="0" t="n">
         <v>0.234</v>
       </c>
       <c r="N11" s="0" t="n">
+        <v>0.128</v>
+      </c>
+      <c r="O11" s="13" t="n">
+        <v>0.194</v>
+      </c>
+      <c r="P11" s="0" t="n">
         <v>0.13</v>
       </c>
-      <c r="O11" s="0" t="n">
+      <c r="Q11" s="0" t="n">
         <v>0.061</v>
       </c>
-      <c r="P11" s="0" t="n">
+      <c r="R11" s="0" t="n">
         <v>0.137</v>
       </c>
-      <c r="Q11" s="0" t="n">
+      <c r="S11" s="0" t="n">
         <v>0.07</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="12" t="n">
         <v>0.063</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>0.125</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="13" t="n">
         <v>0.187</v>
       </c>
       <c r="I12" s="0" t="n">
@@ -1976,128 +2215,148 @@
       <c r="K12" s="0" t="n">
         <v>0.53</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="L12" s="12" t="n">
         <v>0.142</v>
       </c>
       <c r="M12" s="0" t="n">
         <v>0.232</v>
       </c>
       <c r="N12" s="0" t="n">
+        <v>0.107</v>
+      </c>
+      <c r="O12" s="13" t="n">
+        <v>0.199</v>
+      </c>
+      <c r="P12" s="0" t="n">
         <v>0.132</v>
       </c>
-      <c r="O12" s="0" t="n">
+      <c r="Q12" s="0" t="n">
         <v>0.062</v>
       </c>
-      <c r="P12" s="0" t="n">
+      <c r="R12" s="0" t="n">
         <v>0.138</v>
       </c>
-      <c r="Q12" s="0" t="n">
+      <c r="S12" s="0" t="n">
         <v>0.064</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2" t="s">
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2" t="s">
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2" t="s">
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J23" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="K23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="L23" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M23" s="3" t="s">
+      <c r="M23" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N23" s="3" t="s">
+      <c r="N23" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="O23" s="3" t="s">
+      <c r="O23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="P23" s="3" t="s">
+      <c r="P23" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="Q23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R23" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="E24" s="8" t="n">
         <v>869</v>
       </c>
-      <c r="F24" s="3" t="n">
+      <c r="F24" s="6" t="n">
         <v>90</v>
       </c>
-      <c r="G24" s="3" t="n">
+      <c r="G24" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="H24" s="3" t="n">
+      <c r="H24" s="6" t="n">
         <v>3995</v>
       </c>
-      <c r="I24" s="3" t="n">
+      <c r="I24" s="6" t="n">
         <v>5861</v>
       </c>
-      <c r="J24" s="3" t="n">
+      <c r="J24" s="6" t="n">
         <v>6867</v>
       </c>
-      <c r="K24" s="3" t="n">
+      <c r="K24" s="8" t="n">
         <v>1958</v>
       </c>
-      <c r="L24" s="3" t="n">
+      <c r="L24" s="6" t="n">
         <v>554</v>
       </c>
-      <c r="M24" s="3" t="n">
+      <c r="M24" s="6" t="n">
+        <v>1078</v>
+      </c>
+      <c r="N24" s="9" t="n">
+        <v>1637</v>
+      </c>
+      <c r="O24" s="6" t="n">
         <v>5910</v>
       </c>
-      <c r="N24" s="3" t="n">
+      <c r="P24" s="6" t="n">
         <v>9036</v>
       </c>
-      <c r="O24" s="3" t="n">
+      <c r="Q24" s="6" t="n">
         <v>9036</v>
       </c>
-      <c r="P24" s="3" t="n">
+      <c r="R24" s="6" t="n">
         <v>5910</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="12" t="n">
         <f aca="false">AVERAGE(F7:F12)</f>
         <v>0.0633333333333333</v>
       </c>
@@ -2105,7 +2364,7 @@
         <f aca="false">AVERAGE(G7:G12)</f>
         <v>0.124</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="13" t="n">
         <f aca="false">AVERAGE(H7:H12)</f>
         <v>0.189</v>
       </c>
@@ -2121,7 +2380,7 @@
         <f aca="false">AVERAGE(K7:K12)</f>
         <v>0.540833333333333</v>
       </c>
-      <c r="K25" s="0" t="n">
+      <c r="K25" s="12" t="n">
         <f aca="false">AVERAGE(L7:L12)</f>
         <v>0.141</v>
       </c>
@@ -2131,18 +2390,26 @@
       </c>
       <c r="M25" s="0" t="n">
         <f aca="false">AVERAGE(N7:N12)</f>
-        <v>0.133666666666667</v>
-      </c>
-      <c r="N25" s="0" t="n">
+        <v>0.124</v>
+      </c>
+      <c r="N25" s="13" t="n">
         <f aca="false">AVERAGE(O7:O12)</f>
-        <v>0.064</v>
+        <v>0.194</v>
       </c>
       <c r="O25" s="0" t="n">
         <f aca="false">AVERAGE(P7:P12)</f>
-        <v>0.136166666666667</v>
+        <v>0.133666666666667</v>
       </c>
       <c r="P25" s="0" t="n">
         <f aca="false">AVERAGE(Q7:Q12)</f>
+        <v>0.064</v>
+      </c>
+      <c r="Q25" s="0" t="n">
+        <f aca="false">AVERAGE(R7:R12)</f>
+        <v>0.136166666666667</v>
+      </c>
+      <c r="R25" s="0" t="n">
+        <f aca="false">AVERAGE(S7:S12)</f>
         <v>0.065</v>
       </c>
     </row>
@@ -2150,12 +2417,12 @@
   <mergeCells count="8">
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="I4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="P4:S4"/>
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:P22"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="O22:R22"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2173,132 +2440,149 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="F12:R33"/>
+  <dimension ref="F12:T33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M26" activeCellId="0" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="43.1989795918367"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2" t="s">
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2" t="s">
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2" t="s">
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="M13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N13" s="3" t="s">
+      <c r="N13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="O13" s="3" t="s">
+      <c r="O13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P13" s="3" t="s">
+      <c r="P13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="Q13" s="3" t="s">
+      <c r="Q13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="R13" s="3" t="s">
+      <c r="R13" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="S13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T13" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F14" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="G14" s="8" t="n">
         <v>1287</v>
       </c>
-      <c r="H14" s="3" t="n">
+      <c r="H14" s="6" t="n">
         <v>156</v>
       </c>
-      <c r="I14" s="3" t="n">
+      <c r="I14" s="9" t="n">
         <v>34</v>
       </c>
-      <c r="J14" s="3" t="n">
+      <c r="J14" s="6" t="n">
         <v>5864</v>
       </c>
-      <c r="K14" s="3" t="n">
+      <c r="K14" s="6" t="n">
         <v>8481</v>
       </c>
-      <c r="L14" s="3" t="n">
+      <c r="L14" s="6" t="n">
         <v>10035</v>
       </c>
-      <c r="M14" s="3" t="n">
+      <c r="M14" s="8" t="n">
         <v>2944</v>
       </c>
-      <c r="N14" s="3" t="n">
+      <c r="N14" s="6" t="n">
         <v>800</v>
       </c>
-      <c r="O14" s="3" t="n">
+      <c r="O14" s="6" t="n">
+        <v>1547</v>
+      </c>
+      <c r="P14" s="9" t="n">
+        <v>2433</v>
+      </c>
+      <c r="Q14" s="6" t="n">
         <v>8958</v>
       </c>
-      <c r="P14" s="3" t="n">
+      <c r="R14" s="6" t="n">
         <v>13535</v>
       </c>
-      <c r="Q14" s="3" t="n">
+      <c r="S14" s="6" t="n">
         <v>13535</v>
       </c>
-      <c r="R14" s="3" t="n">
+      <c r="T14" s="6" t="n">
         <v>8958</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="12" t="n">
         <v>0.101</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>0.19</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I15" s="13" t="n">
         <v>0.296</v>
       </c>
       <c r="J15" s="0" t="n">
@@ -2310,33 +2594,39 @@
       <c r="L15" s="0" t="n">
         <v>1.026</v>
       </c>
-      <c r="M15" s="0" t="n">
+      <c r="M15" s="12" t="n">
         <v>0.245</v>
       </c>
       <c r="N15" s="0" t="n">
         <v>0.402</v>
       </c>
       <c r="O15" s="0" t="n">
+        <v>0.182</v>
+      </c>
+      <c r="P15" s="13" t="n">
+        <v>0.308</v>
+      </c>
+      <c r="Q15" s="0" t="n">
         <v>0.256</v>
       </c>
-      <c r="P15" s="0" t="n">
+      <c r="R15" s="0" t="n">
         <v>0.101</v>
       </c>
-      <c r="Q15" s="0" t="n">
+      <c r="S15" s="0" t="n">
         <v>0.261</v>
       </c>
-      <c r="R15" s="0" t="n">
+      <c r="T15" s="0" t="n">
         <v>0.106</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="12" t="n">
         <v>0.099</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>0.191</v>
       </c>
-      <c r="I16" s="0" t="n">
+      <c r="I16" s="13" t="n">
         <v>0.299</v>
       </c>
       <c r="J16" s="0" t="n">
@@ -2348,33 +2638,39 @@
       <c r="L16" s="0" t="n">
         <v>1.02</v>
       </c>
-      <c r="M16" s="0" t="n">
+      <c r="M16" s="12" t="n">
         <v>0.248</v>
       </c>
       <c r="N16" s="0" t="n">
         <v>0.402</v>
       </c>
       <c r="O16" s="0" t="n">
+        <v>0.181</v>
+      </c>
+      <c r="P16" s="13" t="n">
+        <v>0.315</v>
+      </c>
+      <c r="Q16" s="0" t="n">
         <v>0.258</v>
       </c>
-      <c r="P16" s="0" t="n">
+      <c r="R16" s="0" t="n">
         <v>0.096</v>
       </c>
-      <c r="Q16" s="0" t="n">
+      <c r="S16" s="0" t="n">
         <v>0.262</v>
       </c>
-      <c r="R16" s="0" t="n">
+      <c r="T16" s="0" t="n">
         <v>0.106</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="12" t="n">
         <v>0.096</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>0.19</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="I17" s="13" t="n">
         <v>0.289</v>
       </c>
       <c r="J17" s="0" t="n">
@@ -2386,33 +2682,39 @@
       <c r="L17" s="0" t="n">
         <v>1.02</v>
       </c>
-      <c r="M17" s="0" t="n">
+      <c r="M17" s="12" t="n">
         <v>0.249</v>
       </c>
       <c r="N17" s="0" t="n">
         <v>0.407</v>
       </c>
       <c r="O17" s="0" t="n">
+        <v>0.181</v>
+      </c>
+      <c r="P17" s="13" t="n">
+        <v>0.299</v>
+      </c>
+      <c r="Q17" s="0" t="n">
         <v>0.259</v>
       </c>
-      <c r="P17" s="0" t="n">
+      <c r="R17" s="0" t="n">
         <v>0.101</v>
       </c>
-      <c r="Q17" s="0" t="n">
+      <c r="S17" s="0" t="n">
         <v>0.261</v>
       </c>
-      <c r="R17" s="0" t="n">
+      <c r="T17" s="0" t="n">
         <v>0.104</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="12" t="n">
         <v>0.098</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>0.191</v>
       </c>
-      <c r="I18" s="0" t="n">
+      <c r="I18" s="13" t="n">
         <v>0.291</v>
       </c>
       <c r="J18" s="0" t="n">
@@ -2424,33 +2726,39 @@
       <c r="L18" s="0" t="n">
         <v>1.021</v>
       </c>
-      <c r="M18" s="0" t="n">
+      <c r="M18" s="12" t="n">
         <v>0.25</v>
       </c>
       <c r="N18" s="0" t="n">
         <v>0.405</v>
       </c>
       <c r="O18" s="0" t="n">
+        <v>0.183</v>
+      </c>
+      <c r="P18" s="13" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="Q18" s="0" t="n">
         <v>0.261</v>
       </c>
-      <c r="P18" s="0" t="n">
+      <c r="R18" s="0" t="n">
         <v>0.096</v>
       </c>
-      <c r="Q18" s="0" t="n">
+      <c r="S18" s="0" t="n">
         <v>0.262</v>
       </c>
-      <c r="R18" s="0" t="n">
+      <c r="T18" s="0" t="n">
         <v>0.104</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="12" t="n">
         <v>0.099</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>0.191</v>
       </c>
-      <c r="I19" s="0" t="n">
+      <c r="I19" s="13" t="n">
         <v>0.292</v>
       </c>
       <c r="J19" s="0" t="n">
@@ -2462,24 +2770,31 @@
       <c r="L19" s="0" t="n">
         <v>1.017</v>
       </c>
-      <c r="M19" s="0" t="n">
+      <c r="M19" s="12" t="n">
         <v>0.245</v>
       </c>
       <c r="N19" s="0" t="n">
         <v>0.405</v>
       </c>
       <c r="O19" s="0" t="n">
+        <v>0.182</v>
+      </c>
+      <c r="P19" s="13" t="n">
+        <v>0.298</v>
+      </c>
+      <c r="Q19" s="0" t="n">
         <v>0.26</v>
       </c>
-      <c r="Q19" s="0" t="n">
+      <c r="S19" s="0" t="n">
         <v>0.27</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="12"/>
       <c r="H20" s="0" t="n">
         <v>0.194</v>
       </c>
-      <c r="I20" s="0" t="n">
+      <c r="I20" s="13" t="n">
         <v>0.288</v>
       </c>
       <c r="J20" s="0" t="n">
@@ -2491,116 +2806,135 @@
       <c r="L20" s="0" t="n">
         <v>1.023</v>
       </c>
+      <c r="M20" s="12"/>
       <c r="N20" s="0" t="n">
         <v>0.406</v>
       </c>
-      <c r="Q20" s="0" t="n">
+      <c r="O20" s="0" t="n">
+        <v>0.186</v>
+      </c>
+      <c r="P20" s="13"/>
+      <c r="S20" s="0" t="n">
         <v>0.259</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2" t="s">
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2" t="s">
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2" t="s">
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="I31" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J31" s="3" t="s">
+      <c r="J31" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K31" s="3" t="s">
+      <c r="K31" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L31" s="3" t="s">
+      <c r="L31" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M31" s="3" t="s">
+      <c r="M31" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N31" s="3" t="s">
+      <c r="N31" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="O31" s="3" t="s">
+      <c r="O31" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P31" s="3" t="s">
+      <c r="P31" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="Q31" s="3" t="s">
+      <c r="Q31" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="R31" s="3" t="s">
+      <c r="R31" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="S31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T31" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F32" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="G32" s="8" t="n">
         <v>1287</v>
       </c>
-      <c r="H32" s="3" t="n">
+      <c r="H32" s="6" t="n">
         <v>156</v>
       </c>
-      <c r="I32" s="3" t="n">
+      <c r="I32" s="9" t="n">
         <v>34</v>
       </c>
-      <c r="J32" s="3" t="n">
+      <c r="J32" s="6" t="n">
         <v>5864</v>
       </c>
-      <c r="K32" s="3" t="n">
+      <c r="K32" s="6" t="n">
         <v>8481</v>
       </c>
-      <c r="L32" s="3" t="n">
+      <c r="L32" s="6" t="n">
         <v>10035</v>
       </c>
-      <c r="M32" s="3" t="n">
+      <c r="M32" s="8" t="n">
         <v>2944</v>
       </c>
-      <c r="N32" s="3" t="n">
+      <c r="N32" s="6" t="n">
         <v>800</v>
       </c>
-      <c r="O32" s="3" t="n">
+      <c r="O32" s="6" t="n">
+        <v>1547</v>
+      </c>
+      <c r="P32" s="9" t="n">
+        <v>2433</v>
+      </c>
+      <c r="Q32" s="6" t="n">
         <v>8958</v>
       </c>
-      <c r="P32" s="3" t="n">
+      <c r="R32" s="6" t="n">
         <v>13535</v>
       </c>
-      <c r="Q32" s="3" t="n">
+      <c r="S32" s="6" t="n">
         <v>13535</v>
       </c>
-      <c r="R32" s="3" t="n">
+      <c r="T32" s="6" t="n">
         <v>8958</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G33" s="0" t="n">
+      <c r="G33" s="12" t="n">
         <f aca="false">AVERAGE(G15:G20)</f>
         <v>0.0986</v>
       </c>
@@ -2608,7 +2942,7 @@
         <f aca="false">AVERAGE(H15:H20)</f>
         <v>0.191166666666667</v>
       </c>
-      <c r="I33" s="0" t="n">
+      <c r="I33" s="13" t="n">
         <f aca="false">AVERAGE(I15:I20)</f>
         <v>0.2925</v>
       </c>
@@ -2624,7 +2958,7 @@
         <f aca="false">AVERAGE(L15:L20)</f>
         <v>1.02116666666667</v>
       </c>
-      <c r="M33" s="0" t="n">
+      <c r="M33" s="12" t="n">
         <f aca="false">AVERAGE(M15:M20)</f>
         <v>0.2474</v>
       </c>
@@ -2634,18 +2968,26 @@
       </c>
       <c r="O33" s="0" t="n">
         <f aca="false">AVERAGE(O15:O20)</f>
-        <v>0.2588</v>
-      </c>
-      <c r="P33" s="0" t="n">
+        <v>0.1825</v>
+      </c>
+      <c r="P33" s="13" t="n">
         <f aca="false">AVERAGE(P15:P20)</f>
-        <v>0.0985</v>
+        <v>0.304</v>
       </c>
       <c r="Q33" s="0" t="n">
         <f aca="false">AVERAGE(Q15:Q20)</f>
-        <v>0.2625</v>
+        <v>0.2588</v>
       </c>
       <c r="R33" s="0" t="n">
         <f aca="false">AVERAGE(R15:R20)</f>
+        <v>0.0985</v>
+      </c>
+      <c r="S33" s="0" t="n">
+        <f aca="false">AVERAGE(S15:S20)</f>
+        <v>0.2625</v>
+      </c>
+      <c r="T33" s="0" t="n">
+        <f aca="false">AVERAGE(T15:T20)</f>
         <v>0.105</v>
       </c>
     </row>
@@ -2653,12 +2995,12 @@
   <mergeCells count="8">
     <mergeCell ref="G12:I12"/>
     <mergeCell ref="J12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:R12"/>
+    <mergeCell ref="M12:P12"/>
+    <mergeCell ref="Q12:T12"/>
     <mergeCell ref="G30:I30"/>
     <mergeCell ref="J30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="O30:R30"/>
+    <mergeCell ref="M30:P30"/>
+    <mergeCell ref="Q30:T30"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
timing for tests changed
</commit_message>
<xml_diff>
--- a/results/datasheets/search-results.xlsx
+++ b/results/datasheets/search-results.xlsx
@@ -5,12 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="5000" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="10000" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="15000" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="client iee server" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="not" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="25">
   <si>
     <t xml:space="preserve">AND</t>
   </si>
@@ -71,6 +73,33 @@
   <si>
     <t xml:space="preserve">returned docs:</t>
   </si>
+  <si>
+    <t xml:space="preserve">client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5000 w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000 w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15000 w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 nots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 nots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 nots</t>
+  </si>
 </sst>
 </file>
 
@@ -79,7 +108,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -107,6 +136,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -321,9 +356,9 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF004586"/>
@@ -339,7 +374,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -362,6 +397,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -473,11 +509,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="82643858"/>
-        <c:axId val="55946521"/>
+        <c:axId val="12872142"/>
+        <c:axId val="16156149"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82643858"/>
+        <c:axId val="12872142"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -512,14 +548,851 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55946521"/>
+        <c:crossAx val="16156149"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55946521"/>
+        <c:axId val="16156149"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="12872142"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0515650932108534"/>
+          <c:y val="0.0613723540275607"/>
+          <c:w val="0.881624146049635"/>
+          <c:h val="0.359283989203012"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'10000'!$E$23:$R$23</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>2 words</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5 words</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10 words</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2 words</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5 words</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10 words</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(call || enron) &amp;&amp; (time || attach)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(call || enron) &amp;&amp; (time || attach) &amp;&amp; (inform || work) &amp;&amp; (meet || week)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(call &amp;&amp; enron) || (time &amp;&amp; attach)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(call &amp;&amp; enron) || (time &amp;&amp; attach) || (inform &amp;&amp; work) || (meet &amp;&amp; week)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>!enron &amp;&amp; !time</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>!(enron &amp;&amp; time)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>!enron || !time</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>!(enron || time)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'10000'!$E$25:$R$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.0633333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.124</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.189</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0646666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2245</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.540833333333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.141</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.234</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.124</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.194</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.133666666666667</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.064</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.136166666666667</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.065</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="35997320"/>
+        <c:axId val="86662728"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="35997320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="86662728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="86662728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="35997320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'15000'!$G$31:$T$31</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>2 words</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5 words</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10 words</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2 words</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5 words</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10 words</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(call || enron) &amp;&amp; (time || attach)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(call || enron) &amp;&amp; (time || attach) &amp;&amp; (inform || work) &amp;&amp; (meet || week)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(call &amp;&amp; enron) || (time &amp;&amp; attach)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(call &amp;&amp; enron) || (time &amp;&amp; attach) || (inform &amp;&amp; work) || (meet &amp;&amp; week)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>!enron &amp;&amp; !time</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>!(enron &amp;&amp; time)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>!enron || !time</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>!(enron || time)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'15000'!$G$33:$T$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.0986</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.191166666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2925</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.105833333333333</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.399666666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.02116666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2474</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4045</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1825</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.304</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2588</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0985</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.2625</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="39633155"/>
+        <c:axId val="71517812"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="39633155"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="71517812"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="71517812"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="39633155"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="line"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'client iee server'!$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>client</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'client iee server'!$C$18:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'client iee server'!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iee</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'client iee server'!$C$19:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.086</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1885</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.30825</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'client iee server'!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>server</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'client iee server'!$C$20:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0478333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.101166666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.163</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="81518364"/>
+        <c:axId val="82511844"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="81518364"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="82511844"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="82511844"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -563,7 +1436,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82643858"/>
+        <c:crossAx val="81518364"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -587,540 +1460,7 @@
       </c:spPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.0515545590433483"/>
-          <c:y val="0.0613723540275607"/>
-          <c:w val="0.881644245142003"/>
-          <c:h val="0.359283989203012"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'10000'!$E$23:$R$23</c:f>
-              <c:strCache>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>2 words</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5 words</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10 words</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2 words</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5 words</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10 words</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>(call || enron) &amp;&amp; (time || attach)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>(call || enron) &amp;&amp; (time || attach) &amp;&amp; (inform || work) &amp;&amp; (meet || week)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>(call &amp;&amp; enron) || (time &amp;&amp; attach)</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>(call &amp;&amp; enron) || (time &amp;&amp; attach) || (inform &amp;&amp; work) || (meet &amp;&amp; week)</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>!enron &amp;&amp; !time</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>!(enron &amp;&amp; time)</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>!enron || !time</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>!(enron || time)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'10000'!$E$25:$R$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0.0633333333333333</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.124</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.189</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0646666666666667</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.2245</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.540833333333333</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.141</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.234</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.124</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.194</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.133666666666667</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.064</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.136166666666667</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.065</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:gapWidth val="100"/>
-        <c:overlap val="0"/>
-        <c:axId val="44984030"/>
-        <c:axId val="7264917"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="44984030"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="7264917"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="7264917"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="44984030"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:plotArea>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'15000'!$G$31:$T$31</c:f>
-              <c:strCache>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>2 words</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5 words</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10 words</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2 words</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5 words</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10 words</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>(call || enron) &amp;&amp; (time || attach)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>(call || enron) &amp;&amp; (time || attach) &amp;&amp; (inform || work) &amp;&amp; (meet || week)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>(call &amp;&amp; enron) || (time &amp;&amp; attach)</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>(call &amp;&amp; enron) || (time &amp;&amp; attach) || (inform &amp;&amp; work) || (meet &amp;&amp; week)</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>!enron &amp;&amp; !time</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>!(enron &amp;&amp; time)</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>!enron || !time</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>!(enron || time)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'15000'!$G$33:$T$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0.0986</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.191166666666667</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.2925</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.105833333333333</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.399666666666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.02116666666667</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.2474</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.4045</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.1825</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.304</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.2588</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.0985</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.2625</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.105</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:gapWidth val="100"/>
-        <c:overlap val="0"/>
-        <c:axId val="52082235"/>
-        <c:axId val="43719508"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="52082235"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="43719508"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="43719508"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="52082235"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
+    <c:dispBlanksAs val="span"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1137,16 +1477,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>609480</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9360</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>93240</xdr:colOff>
+      <xdr:colOff>92880</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>9000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1154,8 +1494,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3895560" y="5855760"/>
-        <a:ext cx="9222120" cy="5695200"/>
+        <a:off x="3342960" y="5855760"/>
+        <a:ext cx="7732080" cy="5694840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1179,9 +1519,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>375840</xdr:colOff>
+      <xdr:colOff>375480</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:rowOff>143280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1189,8 +1529,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3954600" y="4341240"/>
-        <a:ext cx="12042000" cy="5068080"/>
+        <a:off x="3049920" y="4341240"/>
+        <a:ext cx="9326880" cy="5067720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1214,9 +1554,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>349200</xdr:colOff>
+      <xdr:colOff>348840</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>86760</xdr:rowOff>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1224,8 +1564,43 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4615200" y="6112080"/>
-        <a:ext cx="14031360" cy="4541040"/>
+        <a:off x="4538880" y="6112080"/>
+        <a:ext cx="13850280" cy="4540680"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>194760</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>150480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>264960</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>138960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="5884200" y="3076560"/>
+        <a:ext cx="5759640" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1251,9 +1626,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.2551020408163"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="28.2040816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="12" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1855,11 +2233,14 @@
   </sheetPr>
   <dimension ref="D4:S25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F4" s="3" t="s">
@@ -2442,22 +2823,22 @@
   </sheetPr>
   <dimension ref="F12:T33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M26" activeCellId="0" sqref="M26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R33" activeCellId="0" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="7" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="42.25"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3011,4 +3392,564 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:J20"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L11" activeCellId="0" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.086</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0.187</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0.294</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0.152</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.087</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.187</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.358</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.199</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.084</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0.188</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0.101</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.084</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0.103</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0.291</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0.151</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0.083</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0.189</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0.092</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0.053</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>0.103</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <f aca="false">AVERAGE(B4:B9)</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <f aca="false">AVERAGE(E4:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <f aca="false">AVERAGE(H4:H9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <f aca="false">AVERAGE(C4:C9)</f>
+        <v>0.086</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <f aca="false">AVERAGE(F4:F9)</f>
+        <v>0.1885</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <f aca="false">AVERAGE(I4:I7)</f>
+        <v>0.30825</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <f aca="false">AVERAGE(D4:D9)</f>
+        <v>0.0478333333333333</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <f aca="false">AVERAGE(G4:G9)</f>
+        <v>0.101166666666667</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <f aca="false">AVERAGE(J4:J9)</f>
+        <v>0.163</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="H3:P23"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I40" activeCellId="0" sqref="I40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.265</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>0.846</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>0.107</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>0.183</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0.266</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>0.851</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>1.664</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>0.185</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0.264</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0.047</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>0.841</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>1.659</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>0.169</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.267</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>0.841</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>1.664</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>0.176</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>0.848</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>0.101</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>1.658</v>
+      </c>
+      <c r="P9" s="0" t="n">
+        <v>0.179</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0.268</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>0.849</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>0.105</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>1.654</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>0.177</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J21" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <f aca="false">AVERAGE(I5:I10)</f>
+        <v>0.266666666666667</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J22" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <f aca="false">AVERAGE(L5:L10)</f>
+        <v>0.846</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J23" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <f aca="false">AVERAGE(O5:O10)</f>
+        <v>1.6615</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>